<commit_message>
Avance mapeo de chrome
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nahuel De la cruz\Desktop\Nahuel\2 - UiPath Cursos Online\AGRANDDA - INTERNSHIP\CirculateCertification_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C282C759-FC74-4043-BD81-4A6B0D28AF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -123,6 +123,15 @@
   <si>
     <t>OrchestratorAssetFolder</t>
   </si>
+  <si>
+    <t>CirculateCertification_URL</t>
+  </si>
+  <si>
+    <t>https://www.argentina.gob.ar/circular</t>
+  </si>
+  <si>
+    <t>URL to access to the main page</t>
+  </si>
 </sst>
 </file>
 
@@ -173,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -183,6 +192,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -201,7 +211,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -499,11 +509,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
@@ -569,7 +579,17 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1574,7 +1594,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -2682,11 +2702,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>

</xml_diff>